<commit_message>
Lab 2 Wednesday Worksesh Feb 19
</commit_message>
<xml_diff>
--- a/Lab 2/E205_Lab2_NuScenesData.xlsx
+++ b/Lab 2/E205_Lab2_NuScenesData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janechowatts/Desktop/E205/Lab 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163D3ACB-8754-DA48-A07E-4AAB7323C184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F93026-62E7-9041-95E0-15EEE18E0B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1840" windowWidth="14400" windowHeight="17540" xr2:uid="{DA864444-5E00-5448-9391-4E45375BE65B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DA864444-5E00-5448-9391-4E45375BE65B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,6 +118,14 @@
       <color rgb="FF2FFF12"/>
       <name val="Andale Mono"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,9 +148,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,13 +173,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>660400</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
@@ -583,15 +592,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{634FB882-03BE-5C4C-9A34-2128E43C9D53}">
-  <dimension ref="A1:V41"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -640,26 +649,26 @@
       <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2">
         <v>0</v>
       </c>
@@ -683,7 +692,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>0.5</v>
       </c>
@@ -715,7 +724,7 @@
         <v>-1.9767424575286401</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>1</v>
       </c>
@@ -747,7 +756,7 @@
         <v>-1.9767424575286401</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>1.5</v>
       </c>
@@ -779,7 +788,7 @@
         <v>-1.9767424575286401</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:23">
       <c r="A6">
         <v>2</v>
       </c>
@@ -816,11 +825,11 @@
       <c r="R6">
         <v>1618.5519999999999</v>
       </c>
-      <c r="S6">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="T6">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7">
         <v>2.5</v>
       </c>
@@ -867,10 +876,14 @@
         <v>1618.663</v>
       </c>
       <c r="S7">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
+        <f>SQRT(POWER(Q7-Q6,2) + POWER(R7-R6,2))/0.5</f>
+        <v>0.26681079438445832</v>
+      </c>
+      <c r="T7">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8">
         <v>3</v>
       </c>
@@ -917,10 +930,14 @@
         <v>1618.6369999999999</v>
       </c>
       <c r="S8">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
+        <f t="shared" ref="S8:S41" si="0">SQRT(POWER(Q8-Q7,2) + POWER(R8-R7,2))/0.5</f>
+        <v>6.0033324079317496E-2</v>
+      </c>
+      <c r="T8">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9">
         <v>3.5</v>
       </c>
@@ -967,10 +984,14 @@
         <v>1618.665</v>
       </c>
       <c r="S9">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
+        <f t="shared" si="0"/>
+        <v>0.38212563379070874</v>
+      </c>
+      <c r="T9">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1017,10 +1038,14 @@
         <v>1618.4480000000001</v>
       </c>
       <c r="S10">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
+        <f t="shared" si="0"/>
+        <v>0.53921795222315727</v>
+      </c>
+      <c r="T10">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11">
         <v>4.5</v>
       </c>
@@ -1067,10 +1092,14 @@
         <v>1618.2529999999999</v>
       </c>
       <c r="S11">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
+        <f t="shared" si="0"/>
+        <v>0.42078973371542255</v>
+      </c>
+      <c r="T11">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1117,10 +1146,14 @@
         <v>1618.4190000000001</v>
       </c>
       <c r="S12">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
+        <f t="shared" si="0"/>
+        <v>0.42169183060658849</v>
+      </c>
+      <c r="T12">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13">
         <v>5.5</v>
       </c>
@@ -1167,10 +1200,14 @@
         <v>1618.308</v>
       </c>
       <c r="S13">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
+        <f t="shared" si="0"/>
+        <v>0.24108089928507742</v>
+      </c>
+      <c r="T13">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1217,10 +1254,14 @@
         <v>1618.223</v>
       </c>
       <c r="S14">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
+        <f t="shared" si="0"/>
+        <v>0.18164801127464827</v>
+      </c>
+      <c r="T14">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15">
         <v>6.5</v>
       </c>
@@ -1267,10 +1308,14 @@
         <v>1618.249</v>
       </c>
       <c r="S15">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
+        <f t="shared" si="0"/>
+        <v>6.0033324079317496E-2</v>
+      </c>
+      <c r="T15">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16">
         <v>7</v>
       </c>
@@ -1317,10 +1362,14 @@
         <v>1618.1980000000001</v>
       </c>
       <c r="S16">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
+        <f t="shared" si="0"/>
+        <v>0.1183384975397493</v>
+      </c>
+      <c r="T16">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17">
         <v>7.5</v>
       </c>
@@ -1367,10 +1416,14 @@
         <v>1618.115</v>
       </c>
       <c r="S17">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22">
+        <f t="shared" si="0"/>
+        <v>0.21084591530329425</v>
+      </c>
+      <c r="T17">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18">
         <v>8</v>
       </c>
@@ -1417,10 +1470,14 @@
         <v>1618.0319999999999</v>
       </c>
       <c r="S18">
-        <v>-2.0968560166849799</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
+        <f t="shared" si="0"/>
+        <v>0.21084591530315408</v>
+      </c>
+      <c r="T18">
+        <v>-2.0968560166849799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19">
         <v>8.5</v>
       </c>
@@ -1467,19 +1524,23 @@
         <v>1618.029</v>
       </c>
       <c r="S19">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>2.8635642126542543E-2</v>
       </c>
       <c r="T19">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U19">
         <v>686.65599999999995</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:23">
       <c r="A20">
         <v>9</v>
       </c>
@@ -1526,19 +1587,23 @@
         <v>1618.0119999999999</v>
       </c>
       <c r="S20">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>5.4037024344426532E-2</v>
       </c>
       <c r="T20">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U20">
         <v>686.65599999999995</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:23">
       <c r="A21">
         <v>9.5</v>
       </c>
@@ -1585,19 +1650,23 @@
         <v>1618.021</v>
       </c>
       <c r="S21">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>2.1633307652902996E-2</v>
       </c>
       <c r="T21">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U21">
         <v>686.65599999999995</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:23">
       <c r="A22">
         <v>10</v>
       </c>
@@ -1644,19 +1713,23 @@
         <v>1618.0419999999999</v>
       </c>
       <c r="S22">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>4.3174066289762301E-2</v>
       </c>
       <c r="T22">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U22">
         <v>686.65599999999995</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:23">
       <c r="A23">
         <v>10.5</v>
       </c>
@@ -1703,19 +1776,23 @@
         <v>1618.011</v>
       </c>
       <c r="S23">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>9.5015788161607065E-2</v>
       </c>
       <c r="T23">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U23">
         <v>686.65599999999995</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:23">
       <c r="A24">
         <v>11</v>
       </c>
@@ -1762,19 +1839,23 @@
         <v>1618.0360000000001</v>
       </c>
       <c r="S24">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>5.8309518948594943E-2</v>
       </c>
       <c r="T24">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U24">
         <v>686.65599999999995</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:23">
       <c r="A25">
         <v>11.5</v>
       </c>
@@ -1821,19 +1902,23 @@
         <v>1618.0360000000001</v>
       </c>
       <c r="S25">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="T25">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U25">
         <v>686.65599999999995</v>
       </c>
-      <c r="U25">
+      <c r="V25">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:23">
       <c r="A26">
         <v>12</v>
       </c>
@@ -1880,19 +1965,23 @@
         <v>1618.0229999999999</v>
       </c>
       <c r="S26">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>2.95296461206771E-2</v>
       </c>
       <c r="T26">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U26">
         <v>686.65599999999995</v>
       </c>
-      <c r="U26">
+      <c r="V26">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:23">
       <c r="A27">
         <v>12.5</v>
       </c>
@@ -1939,19 +2028,23 @@
         <v>1617.9590000000001</v>
       </c>
       <c r="S27">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>0.1478512766259861</v>
       </c>
       <c r="T27">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U27">
         <v>686.65599999999995</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:23">
       <c r="A28">
         <v>13</v>
       </c>
@@ -1998,19 +2091,23 @@
         <v>1617.9590000000001</v>
       </c>
       <c r="S28">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="T28">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U28">
         <v>686.65599999999995</v>
       </c>
-      <c r="U28">
+      <c r="V28">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V28">
+      <c r="W28">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:23">
       <c r="A29">
         <v>13.5</v>
       </c>
@@ -2048,19 +2145,23 @@
         <v>1617.9590000000001</v>
       </c>
       <c r="S29">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="T29">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U29">
         <v>686.65599999999995</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:23">
       <c r="A30">
         <v>14</v>
       </c>
@@ -2098,19 +2199,23 @@
         <v>1617.9590000000001</v>
       </c>
       <c r="S30">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="T30">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U30">
         <v>686.65599999999995</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:23">
       <c r="A31">
         <v>14.5</v>
       </c>
@@ -2148,19 +2253,23 @@
         <v>1617.9590000000001</v>
       </c>
       <c r="S31">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="T31">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U31">
         <v>686.63099999999997</v>
       </c>
-      <c r="U31">
+      <c r="V31">
         <v>1570.585</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:23">
       <c r="A32">
         <v>15</v>
       </c>
@@ -2198,19 +2307,23 @@
         <v>1617.9770000000001</v>
       </c>
       <c r="S32">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>6.4899922958267561E-2</v>
       </c>
       <c r="T32">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U32">
         <v>686.60599999999999</v>
       </c>
-      <c r="U32">
+      <c r="V32">
         <v>1570.606</v>
       </c>
-      <c r="V32">
+      <c r="W32">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:23">
       <c r="A33">
         <v>15.5</v>
       </c>
@@ -2248,19 +2361,23 @@
         <v>1617.9960000000001</v>
       </c>
       <c r="S33">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>6.7675697262793766E-2</v>
       </c>
       <c r="T33">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U33">
         <v>686.61900000000003</v>
       </c>
-      <c r="U33">
+      <c r="V33">
         <v>1570.595</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:23">
       <c r="A34">
         <v>16</v>
       </c>
@@ -2298,19 +2415,23 @@
         <v>1618.021</v>
       </c>
       <c r="S34">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>5.8309518948204998E-2</v>
       </c>
       <c r="T34">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U34">
         <v>686.63099999999997</v>
       </c>
-      <c r="U34">
+      <c r="V34">
         <v>1570.585</v>
       </c>
-      <c r="V34">
+      <c r="W34">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:23">
       <c r="A35">
         <v>16.5</v>
       </c>
@@ -2348,19 +2469,23 @@
         <v>1617.403</v>
       </c>
       <c r="S35">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>1.429412466714725</v>
       </c>
       <c r="T35">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U35">
         <v>686.64400000000001</v>
       </c>
-      <c r="U35">
+      <c r="V35">
         <v>1570.5740000000001</v>
       </c>
-      <c r="V35">
+      <c r="W35">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:23">
       <c r="A36">
         <v>17</v>
       </c>
@@ -2398,19 +2523,23 @@
         <v>1617.3109999999999</v>
       </c>
       <c r="S36">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>0.18788294228075395</v>
       </c>
       <c r="T36">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U36">
         <v>686.65599999999995</v>
       </c>
-      <c r="U36">
+      <c r="V36">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V36">
+      <c r="W36">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:23">
       <c r="A37">
         <v>17.5</v>
       </c>
@@ -2448,19 +2577,23 @@
         <v>1616.3579999999999</v>
       </c>
       <c r="S37">
-        <v>-2.0968560166849799</v>
+        <f t="shared" si="0"/>
+        <v>2.2036496999295947</v>
       </c>
       <c r="T37">
+        <v>-2.0968560166849799</v>
+      </c>
+      <c r="U37">
         <v>686.65599999999995</v>
       </c>
-      <c r="U37">
+      <c r="V37">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V37">
+      <c r="W37">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:23">
       <c r="A38">
         <v>18</v>
       </c>
@@ -2498,19 +2631,23 @@
         <v>1614.828</v>
       </c>
       <c r="S38">
+        <f t="shared" si="0"/>
+        <v>3.3939098396981446</v>
+      </c>
+      <c r="T38">
         <v>-2.0008629078252902</v>
       </c>
-      <c r="T38">
+      <c r="U38">
         <v>686.65599999999995</v>
       </c>
-      <c r="U38">
+      <c r="V38">
         <v>1570.5630000000001</v>
       </c>
-      <c r="V38">
+      <c r="W38">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="39" spans="1:22">
+    <row r="39" spans="1:23">
       <c r="A39">
         <v>18.5</v>
       </c>
@@ -2548,19 +2685,23 @@
         <v>1613.2349999999999</v>
       </c>
       <c r="S39">
+        <f t="shared" si="0"/>
+        <v>3.393349377827267</v>
+      </c>
+      <c r="T39">
         <v>-1.90486979896561</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <v>686.71500000000003</v>
       </c>
-      <c r="U39">
+      <c r="V39">
         <v>1570.5129999999999</v>
       </c>
-      <c r="V39">
+      <c r="W39">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:23">
       <c r="A40">
         <v>19</v>
       </c>
@@ -2589,19 +2730,23 @@
         <v>1611.4780000000001</v>
       </c>
       <c r="S40">
+        <f t="shared" si="0"/>
+        <v>3.6225123878322161</v>
+      </c>
+      <c r="T40">
         <v>-1.8525099214057801</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <v>686.77300000000002</v>
       </c>
-      <c r="U40">
+      <c r="V40">
         <v>1570.462</v>
       </c>
-      <c r="V40">
+      <c r="W40">
         <v>-0.71251321382388699</v>
       </c>
     </row>
-    <row r="41" spans="1:22">
+    <row r="41" spans="1:23">
       <c r="A41">
         <v>19.5</v>
       </c>
@@ -2630,15 +2775,19 @@
         <v>1609.65</v>
       </c>
       <c r="S41">
+        <f t="shared" si="0"/>
+        <v>3.6953727822778095</v>
+      </c>
+      <c r="T41">
         <v>-1.69543028872629</v>
       </c>
-      <c r="T41">
+      <c r="U41">
         <v>686.83100000000002</v>
       </c>
-      <c r="U41">
+      <c r="V41">
         <v>1570.412</v>
       </c>
-      <c r="V41">
+      <c r="W41">
         <v>-0.71251321382388699</v>
       </c>
     </row>

</xml_diff>